<commit_message>
Updated project requirements spreadsheet
</commit_message>
<xml_diff>
--- a/ProjectRequirementsSpreadsheet.xlsx
+++ b/ProjectRequirementsSpreadsheet.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\university-calgary\ENSF-592\project-p21-group-4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bcatt\Documents\School - MENG Software Engineering\ENSF592\Project\project-p21-group-4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2713D314-D91A-4561-9553-D1F5C9966F5C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E827A6B5-03A0-42FE-A7DF-EDB3BDD3FF5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8334046A-360A-4D1C-BC26-A7DC8E702074}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8334046A-360A-4D1C-BC26-A7DC8E702074}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$27</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>Item</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Objective</t>
   </si>
   <si>
-    <t>Completed (Y/N)</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -132,12 +129,6 @@
     <t>Use your data to create at least one plot using Matplotlib. Save the plot as a .png file and upload to the repository.</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>Stage 3: User Entry</t>
   </si>
   <si>
@@ -153,10 +144,79 @@
     <t>Stage 1: Dataset Selection</t>
   </si>
   <si>
-    <t>Created a function "check_null" for this. This is just a formality as we are using dropna()</t>
-  </si>
-  <si>
-    <t>We have 12 columns if index is also counted</t>
+    <t>Four separate Excel sheets were used.</t>
+  </si>
+  <si>
+    <t>Program does not modify the excel files directly.</t>
+  </si>
+  <si>
+    <t>12 Columns inclusive of indices.</t>
+  </si>
+  <si>
+    <t>See Github Repository folders - UN Custom Data &amp; UN Population Datasets.</t>
+  </si>
+  <si>
+    <t>No information hard-code or copy-paste within the program except column names.</t>
+  </si>
+  <si>
+    <t>No global variables used.</t>
+  </si>
+  <si>
+    <t>Merge is done using "merge_data" method in class Data Analysis.</t>
+  </si>
+  <si>
+    <t>Import is done using "import_data" method in class DataAnalysis.</t>
+  </si>
+  <si>
+    <t>Data is sorted in "merge_data" method (line 192) in class DataAnalysis.</t>
+  </si>
+  <si>
+    <t>Two level column row index is created in "merge_data" method (line 189) in class DataAnalysis.</t>
+  </si>
+  <si>
+    <t>Created  "check_null" method (line 258)for this. This is just a formality as dropna() is used.</t>
+  </si>
+  <si>
+    <t>Option [4] in the user interface allows for two entries to customize aggregate data.</t>
+  </si>
+  <si>
+    <t>Try/Except statements used to handle invalid user entries throughout.</t>
+  </si>
+  <si>
+    <t>Reference item 5.</t>
+  </si>
+  <si>
+    <t>Printed headers and color coding utilized.</t>
+  </si>
+  <si>
+    <t>User can search for information by selection and keywords/criteria.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Describe method used in "print_aggregate_stats" method (line 314) in DataAnalysis class.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Masking operation used in "higher_gdp_than_usa" method (line 418) in DataAnalysis class. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Groupby operation used in "group_by_stats" method (line 328) in DataAnalysis class. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aggregation operation used in "group_by_stats" method (line 328) in DataAnalysis class. </t>
+  </si>
+  <si>
+    <t>Additional columns added in "additional_statistics" method (line 197) in DataAnalysis class.</t>
+  </si>
+  <si>
+    <t>More than two functions/methods used.</t>
+  </si>
+  <si>
+    <t>Pivot Table created (line 508) and printed (line 513) in "pivot_plot" method in DataAnalysis class.</t>
+  </si>
+  <si>
+    <t>Data is exported using "export_dataset" method (line270) in class DataAnalysis.</t>
+  </si>
+  <si>
+    <t>Plots are created using Matplotlib in "pivot_plot" method (line 517 onwards) in class DataAnalysis.</t>
   </si>
 </sst>
 </file>
@@ -180,8 +240,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -222,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -230,29 +290,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -568,28 +619,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49609F29-55D5-4416-AE11-3B5C9B5E8373}">
-  <dimension ref="A1:E27"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:XFD27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.77734375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="21" style="1" customWidth="1"/>
-    <col min="3" max="3" width="75.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="35.77734375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" hidden="1"/>
+    <col min="1" max="1" width="5.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="75" style="1" customWidth="1"/>
+    <col min="4" max="4" width="60.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -597,364 +649,329 @@
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="5">
-        <v>1</v>
-      </c>
-      <c r="B2" s="10" t="s">
+      <c r="D2" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="7" t="s">
+    </row>
+    <row r="5" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
-        <v>2</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="7" t="s">
+      <c r="B5" s="5"/>
+      <c r="C5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
-        <v>3</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="7" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="7" t="s">
+      <c r="B7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
-        <v>5</v>
-      </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="7" t="s">
+      <c r="B8" s="5"/>
+      <c r="C8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
-        <v>6</v>
-      </c>
-      <c r="B7" s="10" t="s">
+      <c r="B9" s="5"/>
+      <c r="C9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
-        <v>7</v>
-      </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="7" t="s">
+      <c r="B10" s="5"/>
+      <c r="C10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
         <v>11</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
-        <v>8</v>
-      </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="7" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
         <v>12</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
-        <v>9</v>
-      </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="7" t="s">
+      <c r="B12" s="5"/>
+      <c r="C12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
         <v>13</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
-        <v>11</v>
-      </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="7" t="s">
+      <c r="B13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
         <v>14</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
-        <v>12</v>
-      </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="7" t="s">
+      <c r="B14" s="5"/>
+      <c r="C14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
         <v>15</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
-        <v>13</v>
-      </c>
-      <c r="B13" s="10" t="s">
+      <c r="B15" s="5"/>
+      <c r="C15" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>16</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>17</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>18</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="7"/>
+    </row>
+    <row r="19" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>19</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>20</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>21</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>22</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>23</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>24</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>25</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>27</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
-        <v>14</v>
-      </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
-        <v>15</v>
-      </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="5">
-        <v>16</v>
-      </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="5">
-        <v>17</v>
-      </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="5">
-        <v>18</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="5">
-        <v>19</v>
-      </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="5">
-        <v>20</v>
-      </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="5">
-        <v>21</v>
-      </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="5">
-        <v>22</v>
-      </c>
-      <c r="B22" s="10"/>
-      <c r="C22" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="5">
-        <v>23</v>
-      </c>
-      <c r="B23" s="10"/>
-      <c r="C23" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="5">
-        <v>24</v>
-      </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="5">
-        <v>25</v>
-      </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="7" t="s">
+      <c r="C26" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A26" s="5">
-        <v>27</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" s="7" t="s">
+      <c r="D26" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>28</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="5">
-        <v>28</v>
-      </c>
-      <c r="B27" s="10"/>
-      <c r="C27" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E27" s="3"/>
+      <c r="D27" s="7" t="s">
+        <v>59</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E27" xr:uid="{306381AC-0912-4238-B931-54683D43D543}"/>
+  <autoFilter ref="A1:D27" xr:uid="{306381AC-0912-4238-B931-54683D43D543}"/>
   <mergeCells count="5">
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="B7:B12"/>
@@ -963,9 +980,10 @@
     <mergeCell ref="B26:B27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="57" orientation="portrait" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;CGroup 4</oddHeader>
+    <oddHeader>&amp;C&amp;"Calibri Light (Headings),Regular"&amp;16Appendix 1</oddHeader>
+    <oddFooter>&amp;CENSF 592 Spring 2021 – Final Project Report&amp;R3</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>